<commit_message>
test file for xlsx import
</commit_message>
<xml_diff>
--- a/Employees.xlsx
+++ b/Employees.xlsx
@@ -1,5 +1,91 @@
 
-<file path=theme/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\EmployeeAttendance\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FE3327-1537-4E14-9FBE-3C076E0E738E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Blah</t>
+  </si>
+  <si>
+    <t>Glah</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -16,7 +102,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -28,7 +114,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -75,23 +161,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -127,23 +196,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -286,9 +338,56 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
-<file path=theme/theme/themeManager.xml><?xml version="1.0" encoding="utf-8"?>
-<a:themeManager xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>5329</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>2453234523</v>
+      </c>
+      <c r="D1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5325</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5325324321</v>
+      </c>
+      <c r="D2">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>